<commit_message>
fixing E:/ to G:;
</commit_message>
<xml_diff>
--- a/data/2025/permits-by-county-2025.xlsx
+++ b/data/2025/permits-by-county-2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://djei.cloud.gov.ie/apps/eDocs/S/ENT218/Files/ENT218-001-2023/Web Stats 2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naughtm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C797CC9-08E3-4778-BD13-1717CAED2F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB26C589-1190-43A0-83EE-9AD550AF8DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="990" windowWidth="19380" windowHeight="11180" xr2:uid="{711F2E15-F26A-451B-B95B-70CDC9A7A6F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{711F2E15-F26A-451B-B95B-70CDC9A7A6F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,17 +134,17 @@
     <t>Wicklow</t>
   </si>
   <si>
-    <t>*figures accurate to 18th April</t>
-  </si>
-  <si>
     <t>No County Entered</t>
+  </si>
+  <si>
+    <t>Antrim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,12 +155,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -188,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -211,50 +205,33 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,452 +568,509 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2FBF4-4443-4927-87BB-258E00D54789}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7">
+        <v>19903</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2234</v>
+      </c>
+      <c r="D3" s="7">
+        <v>12133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>122</v>
+      </c>
+      <c r="C6" s="6">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>301</v>
+      </c>
+      <c r="C7" s="6">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>336</v>
+      </c>
+      <c r="C8" s="6">
+        <v>88</v>
+      </c>
+      <c r="D8" s="6">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1867</v>
+      </c>
+      <c r="C9" s="6">
+        <v>199</v>
+      </c>
+      <c r="D9" s="6">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>309</v>
+      </c>
+      <c r="C10" s="6">
+        <v>45</v>
+      </c>
+      <c r="D10" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9277</v>
+      </c>
+      <c r="C12" s="6">
+        <v>897</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>665</v>
+      </c>
+      <c r="C13" s="6">
+        <v>83</v>
+      </c>
+      <c r="D13" s="6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>355</v>
+      </c>
+      <c r="C14" s="6">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>833</v>
+      </c>
+      <c r="C15" s="6">
+        <v>124</v>
+      </c>
+      <c r="D15" s="6">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>378</v>
+      </c>
+      <c r="C16" s="6">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>139</v>
+      </c>
+      <c r="C17" s="6">
+        <v>52</v>
+      </c>
+      <c r="D17" s="6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>49</v>
+      </c>
+      <c r="C18" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11">
-        <v>11426</v>
-      </c>
-      <c r="C4" s="11">
-        <v>1247</v>
-      </c>
-      <c r="D4" s="11">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="D18" s="6">
         <v>33</v>
       </c>
-      <c r="B5" s="4">
-        <v>37</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
-        <v>88</v>
-      </c>
-      <c r="C6" s="4">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4">
-        <v>153</v>
-      </c>
-      <c r="C7" s="4">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
-        <v>173</v>
-      </c>
-      <c r="C8" s="4">
-        <v>44</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>946</v>
-      </c>
-      <c r="C9" s="4">
-        <v>95</v>
-      </c>
-      <c r="D9" s="4">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1023</v>
+      </c>
+      <c r="C19" s="6">
+        <v>113</v>
+      </c>
+      <c r="D19" s="6">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>90</v>
+      </c>
+      <c r="C20" s="6">
+        <v>15</v>
+      </c>
+      <c r="D20" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
+        <v>296</v>
+      </c>
+      <c r="C21" s="6">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
+        <v>223</v>
+      </c>
+      <c r="C22" s="6">
+        <v>29</v>
+      </c>
+      <c r="D22" s="6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4">
-        <v>145</v>
-      </c>
-      <c r="C10" s="4">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4">
-        <v>5499</v>
-      </c>
-      <c r="C12" s="4">
-        <v>515</v>
-      </c>
-      <c r="D12" s="4">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4">
-        <v>352</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="B23" s="6">
+        <v>831</v>
+      </c>
+      <c r="C23" s="6">
+        <v>142</v>
+      </c>
+      <c r="D23" s="6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>326</v>
+      </c>
+      <c r="C24" s="6">
+        <v>27</v>
+      </c>
+      <c r="D24" s="6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>234</v>
+      </c>
+      <c r="C25" s="6">
+        <v>21</v>
+      </c>
+      <c r="D25" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6">
+        <v>126</v>
+      </c>
+      <c r="C26" s="6">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4">
-        <v>196</v>
-      </c>
-      <c r="C14" s="4">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4">
-        <v>514</v>
-      </c>
-      <c r="C15" s="4">
-        <v>82</v>
-      </c>
-      <c r="D15" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4">
-        <v>209</v>
-      </c>
-      <c r="C16" s="4">
-        <v>12</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4">
-        <v>82</v>
-      </c>
-      <c r="C17" s="4">
-        <v>32</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4">
-        <v>24</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <v>545</v>
-      </c>
-      <c r="C19" s="4">
-        <v>78</v>
-      </c>
-      <c r="D19" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4">
-        <v>59</v>
-      </c>
-      <c r="C20" s="4">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4">
-        <v>221</v>
-      </c>
-      <c r="C21" s="4">
-        <v>19</v>
-      </c>
-      <c r="D21" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4">
-        <v>128</v>
-      </c>
-      <c r="C22" s="4">
-        <v>13</v>
-      </c>
-      <c r="D22" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4">
-        <v>516</v>
-      </c>
-      <c r="C23" s="4">
-        <v>94</v>
-      </c>
-      <c r="D23" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4">
-        <v>176</v>
-      </c>
-      <c r="C24" s="4">
-        <v>12</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4">
-        <v>113</v>
-      </c>
-      <c r="C25" s="4">
-        <v>9</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4">
-        <v>86</v>
-      </c>
-      <c r="C26" s="4">
-        <v>12</v>
-      </c>
-      <c r="D26" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="D26" s="6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4">
-        <v>60</v>
-      </c>
-      <c r="C27" s="4">
-        <v>13</v>
-      </c>
-      <c r="D27" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B27" s="6">
+        <v>143</v>
+      </c>
+      <c r="C27" s="6">
+        <v>42</v>
+      </c>
+      <c r="D27" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4">
-        <v>213</v>
-      </c>
-      <c r="C28" s="4">
-        <v>10</v>
-      </c>
-      <c r="D28" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="B28" s="6">
+        <v>370</v>
+      </c>
+      <c r="C28" s="6">
+        <v>36</v>
+      </c>
+      <c r="D28" s="6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="4">
-        <v>282</v>
-      </c>
-      <c r="C29" s="4">
-        <v>36</v>
-      </c>
-      <c r="D29" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="B29" s="6">
+        <v>488</v>
+      </c>
+      <c r="C29" s="6">
+        <v>49</v>
+      </c>
+      <c r="D29" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="4">
-        <v>159</v>
-      </c>
-      <c r="C30" s="4">
-        <v>27</v>
-      </c>
-      <c r="D30" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="B30" s="6">
+        <v>285</v>
+      </c>
+      <c r="C30" s="6">
+        <v>54</v>
+      </c>
+      <c r="D30" s="6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="4">
-        <v>310</v>
-      </c>
-      <c r="C31" s="4">
-        <v>13</v>
-      </c>
-      <c r="D31" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
+        <v>596</v>
+      </c>
+      <c r="C31" s="6">
+        <v>34</v>
+      </c>
+      <c r="D31" s="6">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="4">
-        <v>139</v>
-      </c>
-      <c r="C32" s="4">
-        <v>11</v>
-      </c>
-      <c r="D32" s="4">
-        <v>5</v>
+      <c r="B32" s="6">
+        <v>240</v>
+      </c>
+      <c r="C32" s="6">
+        <v>26</v>
+      </c>
+      <c r="D32" s="6">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="eDocument" ma:contentTypeID="0x0101000BC94875665D404BB1351B53C41FD2C000E5CBA74D75A77049B177D97877D56E03" ma:contentTypeVersion="163" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="85309ccccff480a81818d539d3482032">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f94102a1-1d6c-4502-ac27-91905b9321dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3659751ca266c6383aa8c59766733bc" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <m02c691f3efa402dab5cbaa8c240a9e7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Statistics</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">9ba6f678-e647-4dac-946a-fcabffeb8025</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">#Reports</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">139e42fd-3e09-4439-bba7-8aeac7f033ff</TermId>
+        </TermInfo>
+      </Terms>
+    </m02c691f3efa402dab5cbaa8c240a9e7>
+    <TaxCatchAll xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Value>8</Value>
+      <Value>5</Value>
+      <Value>10</Value>
+      <Value>1</Value>
+      <Value>7</Value>
+    </TaxCatchAll>
+    <eDocs_FileStatus xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">Live</eDocs_FileStatus>
+    <h1f8bb4843d6459a8b809123185593c7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">218</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d1f665d0-1ea2-48c4-9fae-9dfb881d0110</TermId>
+        </TermInfo>
+      </Terms>
+    </h1f8bb4843d6459a8b809123185593c7>
+    <fbaa881fc4ae443f9fdafbdd527793df xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </fbaa881fc4ae443f9fdafbdd527793df>
+    <_vti_ItemDeclaredRecord xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
+    <nb1b8a72855341e18dd75ce464e281f2 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2023</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">720401db-42e9-4f5b-a7dd-0e2a6af555be</TermId>
+        </TermInfo>
+      </Terms>
+    </nb1b8a72855341e18dd75ce464e281f2>
+    <eDocs_eFileName xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">ENT218-001-2023</eDocs_eFileName>
+    <mbbd3fafa5ab4e5eb8a6a5e099cef439 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Unclassified</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">779752a3-a421-4077-839c-91815f544ae2</TermId>
+        </TermInfo>
+      </Terms>
+    </mbbd3fafa5ab4e5eb8a6a5e099cef439>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="eDocument" ma:contentTypeID="0x0101000BC94875665D404BB1351B53C41FD2C000E5CBA74D75A77049B177D97877D56E03" ma:contentTypeVersion="181" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9aef13b51d858ac71ab25d278c7edb31">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f94102a1-1d6c-4502-ac27-91905b9321dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="992d5dd0ba35d17e896caa4d336a12f8" ns2:_="">
     <xsd:import namespace="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1243,7 +1277,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1252,47 +1286,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <m02c691f3efa402dab5cbaa8c240a9e7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m02c691f3efa402dab5cbaa8c240a9e7>
-    <TaxCatchAll xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Value>5</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <eDocs_FileStatus xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">Live</eDocs_FileStatus>
-    <h1f8bb4843d6459a8b809123185593c7 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">218</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d1f665d0-1ea2-48c4-9fae-9dfb881d0110</TermId>
-        </TermInfo>
-      </Terms>
-    </h1f8bb4843d6459a8b809123185593c7>
-    <fbaa881fc4ae443f9fdafbdd527793df xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </fbaa881fc4ae443f9fdafbdd527793df>
-    <_vti_ItemDeclaredRecord xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
-    <nb1b8a72855341e18dd75ce464e281f2 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </nb1b8a72855341e18dd75ce464e281f2>
-    <eDocs_eFileName xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd" xsi:nil="true"/>
-    <mbbd3fafa5ab4e5eb8a6a5e099cef439 xmlns="f94102a1-1d6c-4502-ac27-91905b9321dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Unclassified</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">779752a3-a421-4077-839c-91815f544ae2</TermId>
-        </TermInfo>
-      </Terms>
-    </mbbd3fafa5ab4e5eb8a6a5e099cef439>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A59B2-55CF-4E9A-ADEC-6D1F626366C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC8B3DB6-0F7A-4B88-9D49-1569BFED611C}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3707964B-8A63-4BFC-AE72-47FB7628B095}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1309,26 +1320,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B630F9CF-D4FF-4CEA-98D4-56CE26D676B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A59B2-55CF-4E9A-ADEC-6D1F626366C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>